<commit_message>
Added some components to display a person's details. Created a Patient Container which will be used later in Consultation form etc. Added a moment library to help with date and time management in the software (make sure to run "npm i"). Fixed an issue in ChangePassword which led to validation error.
</commit_message>
<xml_diff>
--- a/Working Documentation/Database Tables.xlsx
+++ b/Working Documentation/Database Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Documents\PMASD\Working Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9042F0-7DDB-471D-8A01-FE52802CA15F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BEC0F4-0446-4C27-AFE7-FA0F16D8E44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,10 +977,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1569,7 +1569,7 @@
       <c r="D62" t="s">
         <v>180</v>
       </c>
-      <c r="G62" s="10" t="s">
+      <c r="G62" s="11" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1577,13 +1577,13 @@
       <c r="D63" t="s">
         <v>175</v>
       </c>
-      <c r="G63" s="10"/>
+      <c r="G63" s="11"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>182</v>
       </c>
-      <c r="G64" s="10"/>
+      <c r="G64" s="11"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
@@ -1706,7 +1706,7 @@
       <c r="D93" t="s">
         <v>6</v>
       </c>
-      <c r="G93" s="10" t="s">
+      <c r="G93" s="11" t="s">
         <v>218</v>
       </c>
     </row>
@@ -1714,43 +1714,43 @@
       <c r="D94" t="s">
         <v>197</v>
       </c>
-      <c r="G94" s="10"/>
+      <c r="G94" s="11"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D95" t="s">
         <v>199</v>
       </c>
-      <c r="G95" s="10"/>
+      <c r="G95" s="11"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D96" t="s">
         <v>198</v>
       </c>
-      <c r="G96" s="10"/>
+      <c r="G96" s="11"/>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
         <v>200</v>
       </c>
-      <c r="G97" s="10"/>
+      <c r="G97" s="11"/>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
         <v>156</v>
       </c>
-      <c r="G98" s="10"/>
+      <c r="G98" s="11"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
         <v>201</v>
       </c>
-      <c r="G99" s="10"/>
+      <c r="G99" s="11"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
         <v>202</v>
       </c>
-      <c r="G100" s="10"/>
+      <c r="G100" s="11"/>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D102" t="s">
@@ -1853,8 +1853,8 @@
   <dimension ref="A1:K180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,7 +2049,7 @@
         <v>28</v>
       </c>
       <c r="F17" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>22</v>
@@ -3218,14 +3218,14 @@
     <col min="3" max="3" width="81.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added complete Patient redux boilerplate code. Successfully implemented Patient Search, added additional parameters to search on. Modified existing django tables to link to each user.
</commit_message>
<xml_diff>
--- a/Working Documentation/Database Tables.xlsx
+++ b/Working Documentation/Database Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Documents\PMASD\Working Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BEC0F4-0446-4C27-AFE7-FA0F16D8E44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEED0A63-6470-4C6C-913C-9A571283117E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="251">
   <si>
     <t>Model</t>
   </si>
@@ -856,12 +856,21 @@
   <si>
     <t>history</t>
   </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>ForeingKey</t>
+  </si>
+  <si>
+    <t>not required as data reference available in "patient" but makes life easier</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,6 +921,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -948,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -980,6 +996,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1850,11 +1869,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K180"/>
+  <dimension ref="A1:K187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,14 +2161,11 @@
       <c r="C34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>11</v>
+      <c r="D34" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="2">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2157,7 +2173,7 @@
         <v>229</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>7</v>
@@ -2166,479 +2182,478 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C39" s="2" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C40" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="2" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C42" s="2" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C44" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D47" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C48" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="E48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C45" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D45" s="5" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D49" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C49" s="2" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C53" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="2" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C52" s="2" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C56" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D58" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D55" s="7" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D59" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D56" s="7" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D60" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="2">
+      <c r="E60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D57" s="2" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="2">
+      <c r="E61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D58" s="2" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D62" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F62" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="2" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B70" s="2" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B74" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B73" s="2" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D80" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D81" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D77" s="7" t="s">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D82" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D78" s="7" t="s">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D83" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D79" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B83" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="2">
-        <v>50</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D84" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D85" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D86" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D87" s="2" t="s">
-        <v>71</v>
+      <c r="C87" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="2">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D88" s="7" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="E88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D89" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D90" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C91" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D91" s="7" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D92" s="7" t="s">
-        <v>70</v>
+      <c r="D92" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F92" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D93" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C96" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D97" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D98" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F93" s="2">
+      <c r="E98" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F98" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D94" s="2" t="s">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D99" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" s="2">
+      <c r="E99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D95" s="2" t="s">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D100" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F95" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D96" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F96" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D97" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F97" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B100" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
@@ -2646,54 +2661,60 @@
       <c r="F100" s="2">
         <v>50</v>
       </c>
-      <c r="G100" s="2" t="s">
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D101" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D102" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F102" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B105" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D106" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F106" s="2">
+        <v>50</v>
+      </c>
+      <c r="G106" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D101" s="7" t="s">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D107" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F101" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C104" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D105" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F105" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D106" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D107" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>7</v>
@@ -2702,42 +2723,39 @@
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D108" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>130</v>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C110" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C111" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="D111" s="7" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="F111" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D112" s="7" t="s">
-        <v>77</v>
+      <c r="D112" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F112" s="2">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D113" s="2" t="s">
-        <v>85</v>
+      <c r="D113" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>7</v>
@@ -2747,22 +2765,19 @@
       </c>
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D114" s="2" t="s">
-        <v>86</v>
+      <c r="D114" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F114" s="2">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B117" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="C117" s="2" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>68</v>
@@ -2773,46 +2788,43 @@
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D118" s="7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F118" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D119" s="2" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F119" s="2">
-        <v>100</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>135</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D120" s="2" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="F120" s="2">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B123" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>68</v>
@@ -2823,126 +2835,107 @@
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D124" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F124" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D125" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F125" s="2">
+        <v>100</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D126" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E125" s="2" t="s">
+      <c r="E126" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F125" s="2">
+      <c r="F126" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B129" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D130" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F130" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D131" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F131" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="2:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B128" s="2" t="s">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B134" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D128" s="7" t="s">
+      <c r="D134" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D135" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E128" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F128" s="2">
+      <c r="E135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F135" s="2">
         <v>5</v>
       </c>
-      <c r="G128" s="3" t="s">
+      <c r="G135" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D129" s="7" t="s">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D136" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F129" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D130" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F130" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D131" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F131" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D132" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F132" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D133" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F133" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D134" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F134" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D135" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D136" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>7</v>
@@ -2951,248 +2944,325 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D137" s="2" t="s">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D137" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F137" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D138" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F138" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D139" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F139" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D140" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F140" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D141" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F141" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D142" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D143" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F143" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D144" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F137" s="2">
+      <c r="E144" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F144" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D138" s="2" t="s">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D145" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E138" s="2" t="s">
+      <c r="E145" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D139" s="7" t="s">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D146" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E139" s="2" t="s">
+      <c r="E146" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G139" s="2" t="s">
+      <c r="G146" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D140" s="7" t="s">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D147" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E140" s="2" t="s">
+      <c r="E147" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G140" s="2" t="s">
+      <c r="G147" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C143" s="2" t="s">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C150" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D143" s="7" t="s">
+      <c r="D150" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E143" s="2" t="s">
+      <c r="E150" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D144" s="7" t="s">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D151" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D145" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F145" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D146" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F146" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D147" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F147" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D148" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F148" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B151" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D151" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D152" s="7" t="s">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D152" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F152" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D153" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F153" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D154" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F154" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D155" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F155" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B158" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D159" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E152" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F152" s="2">
+      <c r="E159" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F159" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C155" s="2" t="s">
+    <row r="162" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C162" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D155" s="7" t="s">
+      <c r="D162" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E155" s="2" t="s">
+      <c r="E162" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C156" s="2" t="s">
+    <row r="163" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C163" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D156" s="7" t="s">
+      <c r="D163" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E156" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F156" s="2">
+      <c r="E163" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F163" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D157" s="8" t="s">
+    <row r="164" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D164" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E157" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F157" s="2">
+      <c r="E164" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F164" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D158" s="2" t="s">
+    <row r="165" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D165" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E158" s="2" t="s">
+      <c r="E165" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C161" s="2" t="s">
+    <row r="168" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C168" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D161" s="9" t="s">
+      <c r="D168" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E161" s="2" t="s">
+      <c r="E168" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D162" s="7" t="s">
+    <row r="169" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D169" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E162" s="2" t="s">
+      <c r="E169" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F162" s="2">
+      <c r="F169" s="2">
         <v>300</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C165" s="2" t="s">
+    <row r="172" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C172" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D165" s="7" t="s">
+      <c r="D172" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E165" s="2" t="s">
+      <c r="E172" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D166" s="7" t="s">
+    <row r="173" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D173" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E166" s="2" t="s">
+      <c r="E173" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D167" s="7" t="s">
+    <row r="174" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D174" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="E167" s="2" t="s">
+      <c r="E174" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D171" s="2" t="s">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D178" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E171" s="2" t="s">
+      <c r="E178" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="2" t="s">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="2" t="s">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="2" t="s">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="2" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on PatientContainer.js and it's components
</commit_message>
<xml_diff>
--- a/Working Documentation/Database Tables.xlsx
+++ b/Working Documentation/Database Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Documents\PMASD\Working Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEED0A63-6470-4C6C-913C-9A571283117E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A7C789-E203-4A8A-8339-B5681BB76709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="254">
   <si>
     <t>Model</t>
   </si>
@@ -266,15 +266,6 @@
   </si>
   <si>
     <t>consultations</t>
-  </si>
-  <si>
-    <t>assets</t>
-  </si>
-  <si>
-    <t>liabilities</t>
-  </si>
-  <si>
-    <t>reports</t>
   </si>
   <si>
     <t>Consultation</t>
@@ -779,9 +770,6 @@
     <t>opening_balance</t>
   </si>
   <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>misc</t>
   </si>
   <si>
@@ -864,6 +852,27 @@
   </si>
   <si>
     <t>not required as data reference available in "patient" but makes life easier</t>
+  </si>
+  <si>
+    <t>ud_patient_id</t>
+  </si>
+  <si>
+    <t>User defined patient ID</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>OneToOneField</t>
+  </si>
+  <si>
+    <t>Default: 000000</t>
+  </si>
+  <si>
+    <t>last_patient_id</t>
   </si>
 </sst>
 </file>
@@ -994,11 +1003,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1303,7 +1312,7 @@
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1323,42 +1332,42 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F9">
         <v>500</v>
@@ -1366,129 +1375,129 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
         <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
         <v>18</v>
       </c>
       <c r="G25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G29" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
@@ -1496,7 +1505,7 @@
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E35" t="s">
         <v>24</v>
@@ -1507,31 +1516,31 @@
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D43" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G43" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F51">
         <v>100</v>
@@ -1539,7 +1548,7 @@
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F52">
         <v>500</v>
@@ -1547,7 +1556,7 @@
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
@@ -1555,30 +1564,30 @@
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E61" t="s">
         <v>24</v>
@@ -1586,50 +1595,50 @@
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>180</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>185</v>
+        <v>177</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>175</v>
-      </c>
-      <c r="G63" s="11"/>
+        <v>172</v>
+      </c>
+      <c r="G63" s="12"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>182</v>
-      </c>
-      <c r="G64" s="11"/>
+        <v>179</v>
+      </c>
+      <c r="G64" s="12"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D72" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E73" t="s">
         <v>24</v>
@@ -1637,7 +1646,7 @@
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
         <v>24</v>
@@ -1645,25 +1654,25 @@
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.3">
       <c r="G79" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D80" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E80" t="s">
         <v>24</v>
@@ -1671,25 +1680,25 @@
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D86" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E87" t="s">
         <v>24</v>
@@ -1697,7 +1706,7 @@
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E88" t="s">
         <v>31</v>
@@ -1705,12 +1714,12 @@
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E90" t="s">
         <v>31</v>
@@ -1718,83 +1727,83 @@
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
         <v>6</v>
       </c>
-      <c r="G93" s="11" t="s">
-        <v>218</v>
+      <c r="G93" s="12" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
-        <v>197</v>
-      </c>
-      <c r="G94" s="11"/>
+        <v>194</v>
+      </c>
+      <c r="G94" s="12"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D95" t="s">
-        <v>199</v>
-      </c>
-      <c r="G95" s="11"/>
+        <v>196</v>
+      </c>
+      <c r="G95" s="12"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D96" t="s">
-        <v>198</v>
-      </c>
-      <c r="G96" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="G96" s="12"/>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>200</v>
-      </c>
-      <c r="G97" s="11"/>
+        <v>197</v>
+      </c>
+      <c r="G97" s="12"/>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
-        <v>156</v>
-      </c>
-      <c r="G98" s="11"/>
+        <v>153</v>
+      </c>
+      <c r="G98" s="12"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
-        <v>201</v>
-      </c>
-      <c r="G99" s="11"/>
+        <v>198</v>
+      </c>
+      <c r="G99" s="12"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>202</v>
-      </c>
-      <c r="G100" s="11"/>
+        <v>199</v>
+      </c>
+      <c r="G100" s="12"/>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D102" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C105" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D105" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G105" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D106" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D107" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G107" t="s">
         <v>20</v>
@@ -1802,7 +1811,7 @@
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D108" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E108" t="s">
         <v>31</v>
@@ -1810,7 +1819,7 @@
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D109" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E109" t="s">
         <v>31</v>
@@ -1818,7 +1827,7 @@
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D110" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E110" t="s">
         <v>31</v>
@@ -1826,21 +1835,21 @@
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D111" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E111" t="s">
         <v>31</v>
       </c>
       <c r="G111" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D114" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E114" t="s">
         <v>24</v>
@@ -1848,12 +1857,12 @@
     </row>
     <row r="115" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1869,11 +1878,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K187"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1893,7 +1902,7 @@
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1922,7 +1931,7 @@
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1933,7 +1942,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -1989,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -2017,7 +2026,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>6</v>
@@ -2082,7 +2091,7 @@
         <v>31</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,7 +2102,7 @@
         <v>31</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2124,7 +2133,7 @@
         <v>31</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2135,7 +2144,7 @@
         <v>31</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -2162,7 +2171,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>24</v>
@@ -2170,7 +2179,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C35" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>11</v>
@@ -2212,7 +2221,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2234,7 +2243,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C44" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2242,13 +2251,13 @@
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>24</v>
@@ -2256,10 +2265,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C48" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>222</v>
+        <v>225</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>247</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>7</v>
@@ -2267,21 +2276,24 @@
       <c r="F48" s="2">
         <v>6</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D49" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>43</v>
@@ -2298,12 +2310,12 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C53" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>45</v>
@@ -2320,7 +2332,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2328,7 +2340,7 @@
         <v>46</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>50</v>
@@ -2353,7 +2365,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D60" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>7</v>
@@ -2386,7 +2398,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>57</v>
@@ -2406,7 +2418,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>59</v>
@@ -2426,7 +2438,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>60</v>
@@ -2446,10 +2458,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>38</v>
@@ -2466,7 +2478,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>61</v>
@@ -2489,19 +2501,19 @@
         <v>63</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
@@ -2514,7 +2526,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D82" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>18</v>
@@ -2522,7 +2534,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D83" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>31</v>
@@ -2530,7 +2542,7 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D84" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>24</v>
@@ -2538,13 +2550,13 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>24</v>
@@ -2552,7 +2564,7 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D88" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>7</v>
@@ -2563,7 +2575,7 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D89" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>7</v>
@@ -2574,7 +2586,7 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D90" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>31</v>
@@ -2582,7 +2594,7 @@
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D91" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>31</v>
@@ -2590,7 +2602,7 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D92" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>7</v>
@@ -2601,7 +2613,7 @@
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D93" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>31</v>
@@ -2609,10 +2621,10 @@
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C96" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>24</v>
@@ -2620,7 +2632,7 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D97" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
@@ -2631,7 +2643,7 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D98" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
@@ -2642,7 +2654,7 @@
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D99" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>7</v>
@@ -2653,7 +2665,7 @@
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D100" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
@@ -2664,7 +2676,7 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D101" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>7</v>
@@ -2686,21 +2698,21 @@
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D106" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>7</v>
@@ -2709,12 +2721,12 @@
         <v>50</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D107" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>7</v>
@@ -2725,10 +2737,10 @@
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C110" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>24</v>
@@ -2736,7 +2748,7 @@
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D111" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>7</v>
@@ -2747,7 +2759,7 @@
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D112" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>18</v>
@@ -2755,7 +2767,7 @@
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D113" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>7</v>
@@ -2766,21 +2778,21 @@
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D114" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C117" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>24</v>
@@ -2788,7 +2800,7 @@
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D118" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>7</v>
@@ -2799,7 +2811,7 @@
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D119" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>7</v>
@@ -2810,7 +2822,7 @@
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D120" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>7</v>
@@ -2821,13 +2833,13 @@
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B123" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>24</v>
@@ -2835,7 +2847,7 @@
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D124" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>7</v>
@@ -2846,7 +2858,7 @@
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D125" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>7</v>
@@ -2855,7 +2867,7 @@
         <v>100</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.3">
@@ -2871,13 +2883,13 @@
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B129" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>24</v>
@@ -2885,7 +2897,7 @@
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D130" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>7</v>
@@ -2907,13 +2919,13 @@
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B134" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>24</v>
@@ -2921,7 +2933,7 @@
     </row>
     <row r="135" spans="2:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="D135" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>7</v>
@@ -2930,12 +2942,12 @@
         <v>5</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D136" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>7</v>
@@ -2946,7 +2958,7 @@
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D137" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>56</v>
@@ -2957,7 +2969,7 @@
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D138" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>7</v>
@@ -2968,7 +2980,7 @@
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D139" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>7</v>
@@ -2979,7 +2991,7 @@
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D140" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>7</v>
@@ -2990,7 +3002,7 @@
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D141" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>7</v>
@@ -3001,18 +3013,18 @@
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D142" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D143" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>7</v>
@@ -3023,7 +3035,7 @@
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D144" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>7</v>
@@ -3034,40 +3046,40 @@
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D145" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D146" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E146" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G146" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="G146" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D147" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C150" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>24</v>
@@ -3075,7 +3087,7 @@
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D151" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>24</v>
@@ -3083,7 +3095,7 @@
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D152" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>7</v>
@@ -3094,7 +3106,7 @@
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D153" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>7</v>
@@ -3116,7 +3128,7 @@
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D155" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>56</v>
@@ -3127,13 +3139,13 @@
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B158" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>24</v>
@@ -3141,7 +3153,7 @@
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D159" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>7</v>
@@ -3152,10 +3164,10 @@
     </row>
     <row r="162" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C162" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D162" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>24</v>
@@ -3163,10 +3175,10 @@
     </row>
     <row r="163" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C163" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D163" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>7</v>
@@ -3177,7 +3189,7 @@
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D164" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>7</v>
@@ -3188,7 +3200,7 @@
     </row>
     <row r="165" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D165" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>28</v>
@@ -3196,10 +3208,10 @@
     </row>
     <row r="168" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C168" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>24</v>
@@ -3207,7 +3219,7 @@
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D169" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E169" s="2" t="s">
         <v>56</v>
@@ -3218,10 +3230,10 @@
     </row>
     <row r="172" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C172" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D172" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E172" s="2" t="s">
         <v>24</v>
@@ -3229,7 +3241,7 @@
     </row>
     <row r="173" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D173" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>24</v>
@@ -3237,33 +3249,49 @@
     </row>
     <row r="174" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D174" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D178" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E174" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D178" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="E178" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A184" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" s="2" t="s">
-        <v>66</v>
+        <v>219</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D182" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F182" s="2">
+        <v>6</v>
+      </c>
+      <c r="G182" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3290,48 +3318,48 @@
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed patient history frontend and backend. Styling will be done later.
</commit_message>
<xml_diff>
--- a/Working Documentation/Database Tables.xlsx
+++ b/Working Documentation/Database Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARJUN\Documents\PMASD\Working Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A7C789-E203-4A8A-8339-B5681BB76709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A7F77B-4E7C-41B8-96D1-FCECAD9EAF1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="252">
   <si>
     <t>Model</t>
   </si>
@@ -819,12 +819,6 @@
   </si>
   <si>
     <t>To search for a patient on the basis of patient_id, name and mobile numbers</t>
-  </si>
-  <si>
-    <t>&lt;pk&gt;/</t>
-  </si>
-  <si>
-    <t>To retrieve all data related to a patient, both basic and history</t>
   </si>
   <si>
     <t>To retrieve basic data of patient</t>
@@ -1881,8 +1875,8 @@
   <dimension ref="A1:K182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D183" sqref="D183"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2171,7 +2165,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>24</v>
@@ -2257,7 +2251,7 @@
         <v>37</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>24</v>
@@ -2268,7 +2262,7 @@
         <v>225</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>7</v>
@@ -2277,7 +2271,7 @@
         <v>6</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2365,7 +2359,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D60" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>7</v>
@@ -2461,7 +2455,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>38</v>
@@ -2507,13 +2501,13 @@
         <v>64</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
@@ -2556,7 +2550,7 @@
         <v>76</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>24</v>
@@ -2704,10 +2698,10 @@
         <v>79</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.3">
@@ -2925,7 +2919,7 @@
         <v>90</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>24</v>
@@ -3268,21 +3262,21 @@
         <v>219</v>
       </c>
       <c r="B181" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E181" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D182" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>7</v>
@@ -3291,7 +3285,7 @@
         <v>6</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3302,11 +3296,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97019E76-0B8E-44AC-A16B-6E74715B4D41}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3340,26 +3334,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" t="s">
         <v>239</v>
-      </c>
-      <c r="C7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C9" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>